<commit_message>
Funcionando correctamente apuntando al 33
</commit_message>
<xml_diff>
--- a/excel_to_json.xlsx
+++ b/excel_to_json.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\FILESERVER\Usuarios\ldato\Documents\__CAC\___PROGRAMACION\cod_visaciones\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SistVisac\cod_visaciones\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -66,7 +66,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -89,11 +89,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -102,6 +113,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -382,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -426,6 +440,11 @@
       </c>
       <c r="B7" s="3"/>
     </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>59168</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>